<commit_message>
Converted Text to Numbers
MATLAB would not run when the data points were seen at text and not numbers. Corrected this reading so that MATLAB could run.
</commit_message>
<xml_diff>
--- a/data/GRNmap_input_workbooks/14-gene_25-edges_NW_dCIN5_fam_Sigmoid_estimation.xlsx
+++ b/data/GRNmap_input_workbooks/14-gene_25-edges_NW_dCIN5_fam_Sigmoid_estimation.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="13395" windowHeight="9015" firstSheet="8" activeTab="10"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="13395" windowHeight="9015"/>
   </bookViews>
   <sheets>
     <sheet name="production_rates" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="42">
   <si>
     <t>cols regulators/rows targets</t>
   </si>
@@ -149,126 +149,6 @@
   </si>
   <si>
     <t>production_rate</t>
-  </si>
-  <si>
-    <t>-0.383</t>
-  </si>
-  <si>
-    <t>0.2693</t>
-  </si>
-  <si>
-    <t>1.4649</t>
-  </si>
-  <si>
-    <t>-0.7654</t>
-  </si>
-  <si>
-    <t>-1.1456</t>
-  </si>
-  <si>
-    <t>-0.3518</t>
-  </si>
-  <si>
-    <t>0.5869</t>
-  </si>
-  <si>
-    <t>0.0341</t>
-  </si>
-  <si>
-    <t>0.1712</t>
-  </si>
-  <si>
-    <t>-1.463</t>
-  </si>
-  <si>
-    <t>0.3025</t>
-  </si>
-  <si>
-    <t>1.2958</t>
-  </si>
-  <si>
-    <t>1.5911</t>
-  </si>
-  <si>
-    <t>1.2566</t>
-  </si>
-  <si>
-    <t>0.3325</t>
-  </si>
-  <si>
-    <t>0.6703</t>
-  </si>
-  <si>
-    <t>0.7164</t>
-  </si>
-  <si>
-    <t>-0.5489</t>
-  </si>
-  <si>
-    <t>-0.5302</t>
-  </si>
-  <si>
-    <t>0.016</t>
-  </si>
-  <si>
-    <t>1.5125</t>
-  </si>
-  <si>
-    <t>-0.0775</t>
-  </si>
-  <si>
-    <t>-0.522</t>
-  </si>
-  <si>
-    <t>0.4726</t>
-  </si>
-  <si>
-    <t>0.5256</t>
-  </si>
-  <si>
-    <t>-0.3325</t>
-  </si>
-  <si>
-    <t>1.0717</t>
-  </si>
-  <si>
-    <t>-1.9025</t>
-  </si>
-  <si>
-    <t>-0.4406</t>
-  </si>
-  <si>
-    <t>2.5266</t>
-  </si>
-  <si>
-    <t>0.4041</t>
-  </si>
-  <si>
-    <t>0.1802</t>
-  </si>
-  <si>
-    <t>0.8526</t>
-  </si>
-  <si>
-    <t>-0.4332</t>
-  </si>
-  <si>
-    <t>0.3344</t>
-  </si>
-  <si>
-    <t>-1.2684</t>
-  </si>
-  <si>
-    <t>-0.8782</t>
-  </si>
-  <si>
-    <t>-0.9354</t>
-  </si>
-  <si>
-    <t>-0.0589</t>
-  </si>
-  <si>
-    <t>-0.7158</t>
   </si>
   <si>
     <t>estimate_params</t>
@@ -645,8 +525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -948,7 +828,7 @@
     </row>
     <row r="9" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>81</v>
+        <v>41</v>
       </c>
       <c r="B9" s="10">
         <v>0</v>
@@ -956,7 +836,7 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="B10" s="10">
         <v>1</v>
@@ -1139,7 +1019,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -2100,7 +1980,7 @@
   <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2162,11 +2042,11 @@
       <c r="E2" s="6">
         <v>-0.1191</v>
       </c>
-      <c r="F2" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>41</v>
+      <c r="F2" s="10">
+        <v>-0.38300000000000001</v>
+      </c>
+      <c r="G2" s="10">
+        <v>0.26929999999999998</v>
       </c>
       <c r="H2" s="6">
         <v>-7.5700000000000003E-2</v>
@@ -2194,8 +2074,8 @@
       <c r="B3" s="6">
         <v>-0.3155</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>42</v>
+      <c r="C3" s="10">
+        <v>1.4649000000000001</v>
       </c>
       <c r="D3" s="6">
         <v>-0.80289999999999995</v>
@@ -2203,11 +2083,11 @@
       <c r="E3" s="6">
         <v>0.5141</v>
       </c>
-      <c r="F3" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>44</v>
+      <c r="F3" s="10">
+        <v>-0.76539999999999997</v>
+      </c>
+      <c r="G3" s="10">
+        <v>-1.1456</v>
       </c>
       <c r="H3" s="6">
         <v>0.50960000000000005</v>
@@ -2235,8 +2115,8 @@
       <c r="B4" s="6">
         <v>0.96209999999999996</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>45</v>
+      <c r="C4" s="10">
+        <v>-0.3518</v>
       </c>
       <c r="D4" s="6">
         <v>0.31009999999999999</v>
@@ -2244,11 +2124,11 @@
       <c r="E4" s="6">
         <v>-0.15890000000000001</v>
       </c>
-      <c r="F4" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>47</v>
+      <c r="F4" s="10">
+        <v>0.58689999999999998</v>
+      </c>
+      <c r="G4" s="10">
+        <v>3.4099999999999998E-2</v>
       </c>
       <c r="H4" s="6">
         <v>0.48599999999999999</v>
@@ -2276,8 +2156,8 @@
       <c r="B5" s="6">
         <v>6.3299999999999995E-2</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>48</v>
+      <c r="C5" s="10">
+        <v>0.17119999999999999</v>
       </c>
       <c r="D5" s="6">
         <v>-1.9531000000000001</v>
@@ -2285,11 +2165,11 @@
       <c r="E5" s="6">
         <v>-0.21510000000000001</v>
       </c>
-      <c r="F5" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>50</v>
+      <c r="F5" s="10">
+        <v>-1.4630000000000001</v>
+      </c>
+      <c r="G5" s="10">
+        <v>0.30249999999999999</v>
       </c>
       <c r="H5" s="6">
         <v>-2.2646000000000002</v>
@@ -2317,8 +2197,8 @@
       <c r="B6" s="6">
         <v>-0.91690000000000005</v>
       </c>
-      <c r="C6" s="6" t="s">
-        <v>51</v>
+      <c r="C6" s="10">
+        <v>1.2958000000000001</v>
       </c>
       <c r="D6" s="6">
         <v>0.42699999999999999</v>
@@ -2326,11 +2206,11 @@
       <c r="E6" s="6">
         <v>-7.1199999999999999E-2</v>
       </c>
-      <c r="F6" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>53</v>
+      <c r="F6" s="10">
+        <v>1.5911</v>
+      </c>
+      <c r="G6" s="10">
+        <v>1.2565999999999999</v>
       </c>
       <c r="H6" s="6">
         <v>0.39100000000000001</v>
@@ -2358,8 +2238,8 @@
       <c r="B7" s="6">
         <v>9.8199999999999996E-2</v>
       </c>
-      <c r="C7" s="6" t="s">
-        <v>54</v>
+      <c r="C7" s="10">
+        <v>0.33250000000000002</v>
       </c>
       <c r="D7" s="6">
         <v>0.29420000000000002</v>
@@ -2367,11 +2247,11 @@
       <c r="E7" s="6">
         <v>5.2299999999999999E-2</v>
       </c>
-      <c r="F7" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>56</v>
+      <c r="F7" s="10">
+        <v>0.67030000000000001</v>
+      </c>
+      <c r="G7" s="10">
+        <v>0.71640000000000004</v>
       </c>
       <c r="H7" s="6">
         <v>0.33739999999999998</v>
@@ -2399,8 +2279,8 @@
       <c r="B8" s="7">
         <v>0.57640000000000002</v>
       </c>
-      <c r="C8" s="6" t="s">
-        <v>57</v>
+      <c r="C8" s="10">
+        <v>-0.54890000000000005</v>
       </c>
       <c r="D8" s="6">
         <v>0.24909999999999999</v>
@@ -2408,11 +2288,11 @@
       <c r="E8" s="6">
         <v>0.90359999999999996</v>
       </c>
-      <c r="F8" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>59</v>
+      <c r="F8" s="10">
+        <v>-0.5302</v>
+      </c>
+      <c r="G8" s="10">
+        <v>1.6E-2</v>
       </c>
       <c r="H8" s="6">
         <v>-9.9699999999999997E-2</v>
@@ -2440,8 +2320,8 @@
       <c r="B9" s="6">
         <v>0.58789999999999998</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>60</v>
+      <c r="C9" s="10">
+        <v>1.5125</v>
       </c>
       <c r="D9" s="6">
         <v>0.36570000000000003</v>
@@ -2449,11 +2329,11 @@
       <c r="E9" s="6">
         <v>0.68759999999999999</v>
       </c>
-      <c r="F9" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>62</v>
+      <c r="F9" s="10">
+        <v>-7.7499999999999999E-2</v>
+      </c>
+      <c r="G9" s="10">
+        <v>-0.52200000000000002</v>
       </c>
       <c r="H9" s="6">
         <v>0.30730000000000002</v>
@@ -2481,8 +2361,8 @@
       <c r="B10" s="6">
         <v>1.0931999999999999</v>
       </c>
-      <c r="C10" s="6" t="s">
-        <v>63</v>
+      <c r="C10" s="10">
+        <v>0.47260000000000002</v>
       </c>
       <c r="D10" s="6">
         <v>1.1254999999999999</v>
@@ -2490,11 +2370,11 @@
       <c r="E10" s="6">
         <v>0.62629999999999997</v>
       </c>
-      <c r="F10" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>65</v>
+      <c r="F10" s="10">
+        <v>0.52559999999999996</v>
+      </c>
+      <c r="G10" s="10">
+        <v>-0.33250000000000002</v>
       </c>
       <c r="H10" s="6">
         <v>1.6525000000000001</v>
@@ -2522,8 +2402,8 @@
       <c r="B11" s="6">
         <v>1.2589999999999999</v>
       </c>
-      <c r="C11" s="6" t="s">
-        <v>66</v>
+      <c r="C11" s="10">
+        <v>1.0717000000000001</v>
       </c>
       <c r="D11" s="6">
         <v>0.91600000000000004</v>
@@ -2531,11 +2411,11 @@
       <c r="E11" s="6">
         <v>0.80400000000000005</v>
       </c>
-      <c r="F11" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>68</v>
+      <c r="F11" s="10">
+        <v>-1.9025000000000001</v>
+      </c>
+      <c r="G11" s="10">
+        <v>-0.44059999999999999</v>
       </c>
       <c r="H11" s="6">
         <v>0.56589999999999996</v>
@@ -2572,11 +2452,11 @@
       <c r="E12" s="6">
         <v>-0.54890000000000005</v>
       </c>
-      <c r="F12" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>70</v>
+      <c r="F12" s="10">
+        <v>2.5266000000000002</v>
+      </c>
+      <c r="G12" s="10">
+        <v>0.40410000000000001</v>
       </c>
       <c r="H12" s="6">
         <v>2.5700000000000001E-2</v>
@@ -2604,8 +2484,8 @@
       <c r="B13" s="6">
         <v>-0.1331</v>
       </c>
-      <c r="C13" s="6" t="s">
-        <v>71</v>
+      <c r="C13" s="10">
+        <v>0.1802</v>
       </c>
       <c r="D13" s="6">
         <v>-0.32140000000000002</v>
@@ -2613,11 +2493,11 @@
       <c r="E13" s="6">
         <v>-1.8200000000000001E-2</v>
       </c>
-      <c r="F13" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>73</v>
+      <c r="F13" s="10">
+        <v>0.85260000000000002</v>
+      </c>
+      <c r="G13" s="10">
+        <v>-0.43319999999999997</v>
       </c>
       <c r="H13" s="6">
         <v>0.22489999999999999</v>
@@ -2645,8 +2525,8 @@
       <c r="B14" s="6">
         <v>-1.2421</v>
       </c>
-      <c r="C14" s="6" t="s">
-        <v>74</v>
+      <c r="C14" s="10">
+        <v>0.33439999999999998</v>
       </c>
       <c r="D14" s="6">
         <v>-0.73499999999999999</v>
@@ -2654,11 +2534,11 @@
       <c r="E14" s="6">
         <v>0.29349999999999998</v>
       </c>
-      <c r="F14" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>76</v>
+      <c r="F14" s="10">
+        <v>-1.2684</v>
+      </c>
+      <c r="G14" s="10">
+        <v>-0.87819999999999998</v>
       </c>
       <c r="H14" s="6">
         <v>1.0021</v>
@@ -2686,8 +2566,8 @@
       <c r="B15" s="6">
         <v>-1.3433999999999999</v>
       </c>
-      <c r="C15" s="6" t="s">
-        <v>77</v>
+      <c r="C15" s="10">
+        <v>-0.93540000000000001</v>
       </c>
       <c r="D15" s="6">
         <v>-1.7083999999999999</v>
@@ -2695,11 +2575,11 @@
       <c r="E15" s="6">
         <v>-0.28220000000000001</v>
       </c>
-      <c r="F15" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="G15" s="6" t="s">
-        <v>79</v>
+      <c r="F15" s="10">
+        <v>-5.8900000000000001E-2</v>
+      </c>
+      <c r="G15" s="10">
+        <v>-0.71579999999999999</v>
       </c>
       <c r="H15" s="6">
         <v>-0.11550000000000001</v>

</xml_diff>